<commit_message>
:art: CEC results txt to xlsx
</commit_message>
<xml_diff>
--- a/CEC_txt_to_xlsx/OUTPUTS/D10/CEC2017functions-D10__AGEO2_vs_AGEO2var_5.xlsx
+++ b/CEC_txt_to_xlsx/OUTPUTS/D10/CEC2017functions-D10__AGEO2_vs_AGEO2var_5.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>No1</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Std2</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>1 vs 28</t>
   </si>
 </sst>
@@ -60,12 +63,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,7 +86,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -91,7 +148,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,6 +178,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -113,30 +200,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,9 +214,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,73 +228,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -242,25 +238,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,157 +418,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,30 +462,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -507,20 +479,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,151 +509,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -710,7 +706,7 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,20 +1055,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.14166666666667" style="1"/>
-    <col min="2" max="6" width="9.14166666666667" style="2"/>
+    <col min="2" max="6" width="9.25" style="2"/>
     <col min="7" max="7" width="9.14166666666667" style="1"/>
-    <col min="8" max="10" width="9.14166666666667" style="2"/>
-    <col min="11" max="11" width="9.25" style="2"/>
-    <col min="12" max="12" width="9.14166666666667" style="2"/>
+    <col min="8" max="12" width="9.25" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1153,1071 +1147,1109 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>8240</v>
-      </c>
-      <c r="C3" s="2">
-        <v>75100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25400</v>
-      </c>
-      <c r="E3" s="2">
-        <v>27700</v>
-      </c>
-      <c r="F3" s="2">
-        <v>14000</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4">
-        <v>6200</v>
-      </c>
-      <c r="I3" s="4">
-        <v>31300</v>
-      </c>
-      <c r="J3" s="4">
-        <v>18000</v>
-      </c>
-      <c r="K3" s="4">
-        <v>18300</v>
-      </c>
-      <c r="L3" s="4">
-        <v>5930</v>
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0.963</v>
+        <v>8240</v>
       </c>
       <c r="C4" s="2">
-        <v>162</v>
+        <v>75100</v>
       </c>
       <c r="D4" s="2">
-        <v>42.3</v>
+        <v>25400</v>
       </c>
       <c r="E4" s="2">
-        <v>47.1</v>
+        <v>27700</v>
       </c>
       <c r="F4" s="2">
-        <v>37.2</v>
+        <v>14000</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="4">
-        <v>0.537</v>
+        <v>6200</v>
       </c>
       <c r="I4" s="4">
-        <v>35.7</v>
+        <v>31300</v>
       </c>
       <c r="J4" s="4">
-        <v>8.54</v>
+        <v>18000</v>
       </c>
       <c r="K4" s="4">
-        <v>9.98</v>
+        <v>18300</v>
       </c>
       <c r="L4" s="4">
-        <v>5.84</v>
+        <v>5930</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4">
-        <v>6.34</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.963</v>
       </c>
       <c r="C5" s="2">
-        <v>32.4</v>
+        <v>162</v>
       </c>
       <c r="D5" s="2">
-        <v>19.4</v>
+        <v>42.3</v>
       </c>
       <c r="E5" s="2">
-        <v>19.7</v>
+        <v>47.1</v>
       </c>
       <c r="F5" s="2">
-        <v>6.95</v>
+        <v>37.2</v>
       </c>
       <c r="G5" s="1">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>7.19</v>
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.537</v>
       </c>
       <c r="I5" s="4">
-        <v>19</v>
+        <v>35.7</v>
       </c>
       <c r="J5" s="4">
-        <v>13.6</v>
+        <v>8.54</v>
       </c>
       <c r="K5" s="4">
-        <v>13.1</v>
+        <v>9.98</v>
       </c>
       <c r="L5" s="4">
-        <v>3.15</v>
+        <v>5.84</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.575</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>6.34</v>
       </c>
       <c r="C6" s="2">
-        <v>15.4</v>
+        <v>32.4</v>
       </c>
       <c r="D6" s="2">
-        <v>5.09</v>
+        <v>19.4</v>
       </c>
       <c r="E6" s="2">
-        <v>5.11</v>
+        <v>19.7</v>
       </c>
       <c r="F6" s="2">
-        <v>3.54</v>
+        <v>6.95</v>
       </c>
       <c r="G6" s="1">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.0265</v>
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>7.19</v>
       </c>
       <c r="I6" s="4">
-        <v>4.4</v>
+        <v>19</v>
       </c>
       <c r="J6" s="4">
-        <v>1.07</v>
+        <v>13.6</v>
       </c>
       <c r="K6" s="4">
-        <v>1.3</v>
+        <v>13.1</v>
       </c>
       <c r="L6" s="4">
-        <v>0.887</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4">
-        <v>12.8</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.575</v>
       </c>
       <c r="C7" s="2">
-        <v>91.5</v>
+        <v>15.4</v>
       </c>
       <c r="D7" s="2">
-        <v>58.2</v>
+        <v>5.09</v>
       </c>
       <c r="E7" s="2">
-        <v>56.1</v>
+        <v>5.11</v>
       </c>
       <c r="F7" s="2">
-        <v>16.4</v>
+        <v>3.54</v>
       </c>
       <c r="G7" s="1">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2">
-        <v>15.7</v>
+        <v>6</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.0265</v>
       </c>
       <c r="I7" s="4">
-        <v>65</v>
+        <v>4.4</v>
       </c>
       <c r="J7" s="4">
-        <v>38.6</v>
+        <v>1.07</v>
       </c>
       <c r="K7" s="4">
-        <v>37.7</v>
+        <v>1.3</v>
       </c>
       <c r="L7" s="4">
-        <v>9.07</v>
+        <v>0.887</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>5.57</v>
+        <v>12.8</v>
       </c>
       <c r="C8" s="2">
-        <v>47.8</v>
+        <v>91.5</v>
       </c>
       <c r="D8" s="2">
-        <v>28.3</v>
+        <v>58.2</v>
       </c>
       <c r="E8" s="2">
-        <v>28.4</v>
+        <v>56.1</v>
       </c>
       <c r="F8" s="2">
-        <v>9.19</v>
+        <v>16.4</v>
       </c>
       <c r="G8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2">
-        <v>7.4</v>
+        <v>15.7</v>
       </c>
       <c r="I8" s="4">
-        <v>27.1</v>
+        <v>65</v>
       </c>
       <c r="J8" s="4">
-        <v>17.8</v>
+        <v>38.6</v>
       </c>
       <c r="K8" s="4">
-        <v>17.1</v>
+        <v>37.7</v>
       </c>
       <c r="L8" s="4">
-        <v>4.1</v>
+        <v>9.07</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.839</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5.57</v>
       </c>
       <c r="C9" s="2">
-        <v>914</v>
+        <v>47.8</v>
       </c>
       <c r="D9" s="2">
-        <v>124</v>
+        <v>28.3</v>
       </c>
       <c r="E9" s="2">
-        <v>203</v>
+        <v>28.4</v>
       </c>
       <c r="F9" s="2">
-        <v>199</v>
+        <v>9.19</v>
       </c>
       <c r="G9" s="1">
-        <v>9</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.515</v>
+        <v>8</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.4</v>
       </c>
       <c r="I9" s="4">
-        <v>58.5</v>
+        <v>27.1</v>
       </c>
       <c r="J9" s="4">
-        <v>10.5</v>
+        <v>17.8</v>
       </c>
       <c r="K9" s="4">
-        <v>15.5</v>
+        <v>17.1</v>
       </c>
       <c r="L9" s="4">
-        <v>16.2</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>287</v>
+        <v>0.839</v>
       </c>
       <c r="C10" s="2">
-        <v>1190</v>
+        <v>914</v>
       </c>
       <c r="D10" s="2">
-        <v>761</v>
+        <v>124</v>
       </c>
       <c r="E10" s="2">
-        <v>738</v>
+        <v>203</v>
       </c>
       <c r="F10" s="2">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="G10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="4">
-        <v>150</v>
+        <v>0.515</v>
       </c>
       <c r="I10" s="4">
-        <v>976</v>
+        <v>58.5</v>
       </c>
       <c r="J10" s="4">
-        <v>495</v>
+        <v>10.5</v>
       </c>
       <c r="K10" s="4">
-        <v>495</v>
+        <v>15.5</v>
       </c>
       <c r="L10" s="4">
-        <v>157</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="C11" s="2">
-        <v>22800</v>
+        <v>1190</v>
       </c>
       <c r="D11" s="2">
-        <v>3140</v>
+        <v>761</v>
       </c>
       <c r="E11" s="2">
-        <v>3780</v>
+        <v>738</v>
       </c>
       <c r="F11" s="2">
-        <v>5240</v>
+        <v>233</v>
       </c>
       <c r="G11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4">
-        <v>11.1</v>
+        <v>150</v>
       </c>
       <c r="I11" s="4">
-        <v>4420</v>
+        <v>976</v>
       </c>
       <c r="J11" s="4">
-        <v>72</v>
+        <v>495</v>
       </c>
       <c r="K11" s="4">
-        <v>217</v>
+        <v>495</v>
       </c>
       <c r="L11" s="4">
-        <v>626</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>33000</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
-        <v>371000000</v>
+        <v>22800</v>
       </c>
       <c r="D12" s="2">
-        <v>2790000</v>
+        <v>3140</v>
       </c>
       <c r="E12" s="2">
-        <v>35900000</v>
+        <v>3780</v>
       </c>
       <c r="F12" s="2">
-        <v>89300000</v>
+        <v>5240</v>
       </c>
       <c r="G12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="4">
-        <v>5790</v>
+        <v>11.1</v>
       </c>
       <c r="I12" s="4">
-        <v>5150000</v>
+        <v>4420</v>
       </c>
       <c r="J12" s="4">
-        <v>583000</v>
+        <v>72</v>
       </c>
       <c r="K12" s="4">
-        <v>848000</v>
+        <v>217</v>
       </c>
       <c r="L12" s="4">
-        <v>1010000</v>
+        <v>626</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>73.7</v>
+        <v>33000</v>
       </c>
       <c r="C13" s="2">
-        <v>587000000</v>
+        <v>371000000</v>
       </c>
       <c r="D13" s="2">
-        <v>69800</v>
+        <v>2790000</v>
       </c>
       <c r="E13" s="2">
-        <v>29900000</v>
+        <v>35900000</v>
       </c>
       <c r="F13" s="2">
-        <v>93000000</v>
+        <v>89300000</v>
       </c>
       <c r="G13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="4">
-        <v>55.7</v>
+        <v>5790</v>
       </c>
       <c r="I13" s="4">
-        <v>7560000</v>
+        <v>5150000</v>
       </c>
       <c r="J13" s="4">
-        <v>4330</v>
+        <v>583000</v>
       </c>
       <c r="K13" s="4">
-        <v>158000</v>
+        <v>848000</v>
       </c>
       <c r="L13" s="4">
-        <v>1070000</v>
+        <v>1010000</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>65.2</v>
+        <v>73.7</v>
       </c>
       <c r="C14" s="2">
-        <v>339000000</v>
+        <v>587000000</v>
       </c>
       <c r="D14" s="2">
-        <v>7550</v>
+        <v>69800</v>
       </c>
       <c r="E14" s="2">
-        <v>27800000</v>
+        <v>29900000</v>
       </c>
       <c r="F14" s="2">
-        <v>92800000</v>
+        <v>93000000</v>
       </c>
       <c r="G14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4">
-        <v>14.8</v>
+        <v>55.7</v>
       </c>
       <c r="I14" s="4">
-        <v>1570</v>
+        <v>7560000</v>
       </c>
       <c r="J14" s="4">
-        <v>98</v>
+        <v>4330</v>
       </c>
       <c r="K14" s="4">
-        <v>247</v>
+        <v>158000</v>
       </c>
       <c r="L14" s="4">
-        <v>350</v>
+        <v>1070000</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>7.11</v>
+        <v>65.2</v>
       </c>
       <c r="C15" s="2">
-        <v>33600000</v>
+        <v>339000000</v>
       </c>
       <c r="D15" s="2">
-        <v>1410</v>
+        <v>7550</v>
       </c>
       <c r="E15" s="2">
-        <v>1400000</v>
+        <v>27800000</v>
       </c>
       <c r="F15" s="2">
-        <v>6640000</v>
+        <v>92800000</v>
       </c>
       <c r="G15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="4">
-        <v>6.98</v>
+        <v>14.8</v>
       </c>
       <c r="I15" s="4">
-        <v>1420</v>
+        <v>1570</v>
       </c>
       <c r="J15" s="4">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="K15" s="4">
-        <v>337</v>
+        <v>247</v>
       </c>
       <c r="L15" s="4">
-        <v>341</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>12.5</v>
+        <v>7.11</v>
       </c>
       <c r="C16" s="2">
-        <v>892</v>
+        <v>33600000</v>
       </c>
       <c r="D16" s="2">
-        <v>269</v>
+        <v>1410</v>
       </c>
       <c r="E16" s="2">
-        <v>280</v>
+        <v>1400000</v>
       </c>
       <c r="F16" s="2">
-        <v>186</v>
+        <v>6640000</v>
       </c>
       <c r="G16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="4">
-        <v>1.41</v>
+        <v>6.98</v>
       </c>
       <c r="I16" s="4">
-        <v>279</v>
+        <v>1420</v>
       </c>
       <c r="J16" s="4">
-        <v>50.6</v>
+        <v>175</v>
       </c>
       <c r="K16" s="4">
-        <v>79</v>
+        <v>337</v>
       </c>
       <c r="L16" s="4">
-        <v>75.8</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>18.9</v>
+        <v>12.5</v>
       </c>
       <c r="C17" s="2">
-        <v>566</v>
+        <v>892</v>
       </c>
       <c r="D17" s="2">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="E17" s="2">
-        <v>236</v>
+        <v>280</v>
       </c>
       <c r="F17" s="2">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="G17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="4">
-        <v>6.27</v>
+        <v>1.41</v>
       </c>
       <c r="I17" s="4">
-        <v>57.6</v>
+        <v>279</v>
       </c>
       <c r="J17" s="4">
-        <v>27.2</v>
+        <v>50.6</v>
       </c>
       <c r="K17" s="4">
-        <v>28.5</v>
+        <v>79</v>
       </c>
       <c r="L17" s="4">
-        <v>13.6</v>
+        <v>75.8</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1">
-        <v>18</v>
-      </c>
-      <c r="B18" s="4">
-        <v>106</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>18.9</v>
       </c>
       <c r="C18" s="2">
-        <v>59000000</v>
+        <v>566</v>
       </c>
       <c r="D18" s="2">
-        <v>9290</v>
+        <v>252</v>
       </c>
       <c r="E18" s="2">
-        <v>2380000</v>
+        <v>236</v>
       </c>
       <c r="F18" s="2">
-        <v>11700000</v>
+        <v>152</v>
       </c>
       <c r="G18" s="1">
-        <v>18</v>
-      </c>
-      <c r="H18" s="2">
-        <v>329</v>
+        <v>17</v>
+      </c>
+      <c r="H18" s="4">
+        <v>6.27</v>
       </c>
       <c r="I18" s="4">
-        <v>12900</v>
+        <v>57.6</v>
       </c>
       <c r="J18" s="4">
-        <v>2710</v>
+        <v>27.2</v>
       </c>
       <c r="K18" s="4">
-        <v>3510</v>
+        <v>28.5</v>
       </c>
       <c r="L18" s="4">
-        <v>2470</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.95</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>106</v>
       </c>
       <c r="C19" s="2">
-        <v>249000000</v>
+        <v>59000000</v>
       </c>
       <c r="D19" s="2">
-        <v>2810</v>
+        <v>9290</v>
       </c>
       <c r="E19" s="2">
-        <v>5000000</v>
+        <v>2380000</v>
       </c>
       <c r="F19" s="2">
-        <v>35200000</v>
+        <v>11700000</v>
       </c>
       <c r="G19" s="1">
-        <v>19</v>
-      </c>
-      <c r="H19" s="4">
-        <v>3.77</v>
+        <v>18</v>
+      </c>
+      <c r="H19" s="2">
+        <v>329</v>
       </c>
       <c r="I19" s="4">
-        <v>2430</v>
+        <v>12900</v>
       </c>
       <c r="J19" s="4">
-        <v>50.2</v>
+        <v>2710</v>
       </c>
       <c r="K19" s="4">
-        <v>187</v>
+        <v>3510</v>
       </c>
       <c r="L19" s="4">
-        <v>420</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>59</v>
+        <v>3.95</v>
       </c>
       <c r="C20" s="2">
-        <v>622</v>
+        <v>249000000</v>
       </c>
       <c r="D20" s="2">
-        <v>215</v>
+        <v>2810</v>
       </c>
       <c r="E20" s="2">
-        <v>250</v>
+        <v>5000000</v>
       </c>
       <c r="F20" s="2">
-        <v>132</v>
+        <v>35200000</v>
       </c>
       <c r="G20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="4">
-        <v>2.94</v>
+        <v>3.77</v>
       </c>
       <c r="I20" s="4">
-        <v>68</v>
+        <v>2430</v>
       </c>
       <c r="J20" s="4">
-        <v>24.1</v>
+        <v>50.2</v>
       </c>
       <c r="K20" s="4">
-        <v>26.7</v>
+        <v>187</v>
       </c>
       <c r="L20" s="4">
-        <v>14.9</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4">
-        <v>113</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>59</v>
       </c>
       <c r="C21" s="2">
-        <v>253</v>
+        <v>622</v>
       </c>
       <c r="D21" s="2">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E21" s="2">
-        <v>213</v>
+        <v>250</v>
       </c>
       <c r="F21" s="2">
-        <v>33.7</v>
+        <v>132</v>
       </c>
       <c r="G21" s="1">
-        <v>21</v>
-      </c>
-      <c r="H21" s="2">
-        <v>140</v>
+        <v>20</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2.94</v>
       </c>
       <c r="I21" s="4">
-        <v>223</v>
+        <v>68</v>
       </c>
       <c r="J21" s="4">
-        <v>216</v>
-      </c>
-      <c r="K21" s="5">
-        <v>212</v>
+        <v>24.1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>26.7</v>
       </c>
       <c r="L21" s="4">
-        <v>13.4</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>61.2</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>113</v>
       </c>
       <c r="C22" s="2">
-        <v>1510</v>
+        <v>253</v>
       </c>
       <c r="D22" s="2">
-        <v>303</v>
+        <v>224</v>
       </c>
       <c r="E22" s="2">
-        <v>561</v>
+        <v>213</v>
       </c>
       <c r="F22" s="2">
-        <v>453</v>
+        <v>33.7</v>
       </c>
       <c r="G22" s="1">
-        <v>22</v>
-      </c>
-      <c r="H22" s="4">
-        <v>44.8</v>
+        <v>21</v>
+      </c>
+      <c r="H22" s="2">
+        <v>140</v>
       </c>
       <c r="I22" s="4">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="J22" s="4">
-        <v>123</v>
+        <v>216</v>
       </c>
       <c r="K22" s="4">
-        <v>122</v>
+        <v>212</v>
       </c>
       <c r="L22" s="4">
-        <v>22.7</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>313</v>
+        <v>61.2</v>
       </c>
       <c r="C23" s="2">
-        <v>474</v>
+        <v>1510</v>
       </c>
       <c r="D23" s="2">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="E23" s="2">
-        <v>332</v>
-      </c>
-      <c r="F23" s="4">
-        <v>31.5</v>
+        <v>561</v>
+      </c>
+      <c r="F23" s="2">
+        <v>453</v>
       </c>
       <c r="G23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H23" s="4">
-        <v>85.7</v>
+        <v>44.8</v>
       </c>
       <c r="I23" s="4">
-        <v>324</v>
+        <v>197</v>
       </c>
       <c r="J23" s="4">
-        <v>318</v>
+        <v>123</v>
       </c>
       <c r="K23" s="4">
-        <v>312</v>
-      </c>
-      <c r="L23" s="2">
-        <v>32.9</v>
+        <v>122</v>
+      </c>
+      <c r="L23" s="4">
+        <v>22.7</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4">
-        <v>156</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>313</v>
       </c>
       <c r="C24" s="2">
-        <v>381</v>
+        <v>474</v>
       </c>
       <c r="D24" s="2">
-        <v>355</v>
-      </c>
-      <c r="E24" s="4">
-        <v>316</v>
-      </c>
-      <c r="F24" s="2">
-        <v>72.2</v>
+        <v>325</v>
+      </c>
+      <c r="E24" s="2">
+        <v>332</v>
+      </c>
+      <c r="F24" s="4">
+        <v>31.5</v>
       </c>
       <c r="G24" s="1">
-        <v>24</v>
-      </c>
-      <c r="H24" s="2">
-        <v>213</v>
+        <v>23</v>
+      </c>
+      <c r="H24" s="4">
+        <v>85.7</v>
       </c>
       <c r="I24" s="4">
-        <v>357</v>
+        <v>324</v>
       </c>
       <c r="J24" s="4">
-        <v>348</v>
-      </c>
-      <c r="K24" s="2">
-        <v>340</v>
-      </c>
-      <c r="L24" s="4">
-        <v>29.2</v>
+        <v>318</v>
+      </c>
+      <c r="K24" s="4">
+        <v>312</v>
+      </c>
+      <c r="L24" s="2">
+        <v>32.9</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2">
-        <v>406</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>156</v>
       </c>
       <c r="C25" s="2">
-        <v>637</v>
+        <v>381</v>
       </c>
       <c r="D25" s="2">
-        <v>483</v>
-      </c>
-      <c r="E25" s="2">
-        <v>489</v>
+        <v>355</v>
+      </c>
+      <c r="E25" s="4">
+        <v>316</v>
       </c>
       <c r="F25" s="2">
-        <v>53.3</v>
+        <v>72.2</v>
       </c>
       <c r="G25" s="1">
-        <v>25</v>
-      </c>
-      <c r="H25" s="4">
-        <v>287</v>
+        <v>24</v>
+      </c>
+      <c r="H25" s="2">
+        <v>213</v>
       </c>
       <c r="I25" s="4">
-        <v>462</v>
+        <v>357</v>
       </c>
       <c r="J25" s="4">
-        <v>428</v>
-      </c>
-      <c r="K25" s="4">
-        <v>428</v>
+        <v>348</v>
+      </c>
+      <c r="K25" s="2">
+        <v>340</v>
       </c>
       <c r="L25" s="4">
-        <v>26</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>406</v>
+      </c>
+      <c r="C26" s="2">
+        <v>637</v>
+      </c>
+      <c r="D26" s="2">
+        <v>483</v>
+      </c>
+      <c r="E26" s="2">
+        <v>489</v>
+      </c>
+      <c r="F26" s="2">
+        <v>53.3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>25</v>
+      </c>
+      <c r="H26" s="4">
+        <v>287</v>
+      </c>
+      <c r="I26" s="4">
+        <v>462</v>
+      </c>
+      <c r="J26" s="4">
+        <v>428</v>
+      </c>
+      <c r="K26" s="4">
+        <v>428</v>
+      </c>
+      <c r="L26" s="4">
         <v>26</v>
-      </c>
-      <c r="B26" s="2">
-        <v>218</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1700</v>
-      </c>
-      <c r="D26" s="2">
-        <v>686</v>
-      </c>
-      <c r="E26" s="2">
-        <v>825</v>
-      </c>
-      <c r="F26" s="2">
-        <v>440</v>
-      </c>
-      <c r="G26" s="1">
-        <v>26</v>
-      </c>
-      <c r="H26" s="4">
-        <v>86.5</v>
-      </c>
-      <c r="I26" s="4">
-        <v>761</v>
-      </c>
-      <c r="J26" s="4">
-        <v>418</v>
-      </c>
-      <c r="K26" s="4">
-        <v>414</v>
-      </c>
-      <c r="L26" s="4">
-        <v>96.8</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>393</v>
+        <v>218</v>
       </c>
       <c r="C27" s="2">
-        <v>498</v>
+        <v>1700</v>
       </c>
       <c r="D27" s="2">
-        <v>407</v>
+        <v>686</v>
       </c>
       <c r="E27" s="2">
-        <v>419</v>
+        <v>825</v>
       </c>
       <c r="F27" s="2">
-        <v>27.2</v>
+        <v>440</v>
       </c>
       <c r="G27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H27" s="4">
-        <v>389</v>
+        <v>86.5</v>
       </c>
       <c r="I27" s="4">
-        <v>404</v>
+        <v>761</v>
       </c>
       <c r="J27" s="4">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="K27" s="4">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="L27" s="4">
-        <v>2.95</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="C28" s="2">
-        <v>941</v>
+        <v>498</v>
       </c>
       <c r="D28" s="2">
-        <v>613</v>
+        <v>407</v>
       </c>
       <c r="E28" s="2">
-        <v>594</v>
+        <v>419</v>
       </c>
       <c r="F28" s="2">
-        <v>138</v>
+        <v>27.2</v>
       </c>
       <c r="G28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" s="4">
-        <v>319</v>
+        <v>389</v>
       </c>
       <c r="I28" s="4">
-        <v>613</v>
+        <v>404</v>
       </c>
       <c r="J28" s="4">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="K28" s="4">
-        <v>467</v>
+        <v>398</v>
       </c>
       <c r="L28" s="4">
-        <v>78.6</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>248</v>
+        <v>350</v>
       </c>
       <c r="C29" s="2">
-        <v>538</v>
+        <v>941</v>
       </c>
       <c r="D29" s="2">
-        <v>325</v>
+        <v>613</v>
       </c>
       <c r="E29" s="2">
-        <v>335</v>
+        <v>594</v>
       </c>
       <c r="F29" s="2">
-        <v>54.4</v>
+        <v>138</v>
       </c>
       <c r="G29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H29" s="4">
-        <v>200</v>
+        <v>319</v>
       </c>
       <c r="I29" s="4">
-        <v>420</v>
+        <v>613</v>
       </c>
       <c r="J29" s="4">
-        <v>317</v>
+        <v>447</v>
       </c>
       <c r="K29" s="4">
-        <v>314</v>
+        <v>467</v>
       </c>
       <c r="L29" s="4">
-        <v>50.5</v>
+        <v>78.6</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>248</v>
+      </c>
+      <c r="C30" s="2">
+        <v>538</v>
+      </c>
+      <c r="D30" s="2">
+        <v>325</v>
+      </c>
+      <c r="E30" s="2">
+        <v>335</v>
+      </c>
+      <c r="F30" s="2">
+        <v>54.4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>29</v>
+      </c>
+      <c r="H30" s="4">
+        <v>200</v>
+      </c>
+      <c r="I30" s="4">
+        <v>420</v>
+      </c>
+      <c r="J30" s="4">
+        <v>317</v>
+      </c>
+      <c r="K30" s="4">
+        <v>314</v>
+      </c>
+      <c r="L30" s="4">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B31" s="4">
         <v>8800</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>2550000</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <v>666000</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E31" s="2">
         <v>806000</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F31" s="2">
         <v>674000</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G31" s="1">
         <v>30</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H31" s="2">
         <v>15000</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I31" s="4">
         <v>2280000</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J31" s="4">
         <v>643000</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K31" s="4">
         <v>726000</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L31" s="4">
         <v>537000</v>
       </c>
     </row>
-    <row r="32" spans="7:7">
-      <c r="G32" s="1" t="s">
-        <v>12</v>
+    <row r="33" spans="7:7">
+      <c r="G33" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>